<commit_message>
update learners and to nnls
</commit_message>
<xml_diff>
--- a/model_datamaps/sub_DECODER_covariate_map_v2.xlsx
+++ b/model_datamaps/sub_DECODER_covariate_map_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickbrazeau/Documents/GitHub/VivID_Epi/model_datamaps/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90F13EFC-577E-7745-9193-F19B60A0FB80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D32C264-8EE2-FF4C-84C4-341A66B1BD26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="17220" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="113">
   <si>
     <t>pfldhct_cont</t>
   </si>
@@ -81,12 +81,6 @@
     <t>hv246_fctb</t>
   </si>
   <si>
-    <t>hv014_cont</t>
-  </si>
-  <si>
-    <t>hv014_cont_scale</t>
-  </si>
-  <si>
     <t>hv009_cont</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>Owns Livestock</t>
   </si>
   <si>
-    <t>Number of Children Under 5</t>
-  </si>
-  <si>
     <t>Number of Household Members</t>
   </si>
   <si>
@@ -328,9 +319,6 @@
   </si>
   <si>
     <t>Livestock Ownership</t>
-  </si>
-  <si>
-    <t>Num. Children &lt;5</t>
   </si>
   <si>
     <t>Num. House-Members</t>
@@ -643,10 +631,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G48" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:G48" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:G51">
-    <sortCondition ref="D1:D51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G46" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:G46" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:G49">
+    <sortCondition ref="D1:D49"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="column_name"/>
@@ -958,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO48"/>
+  <dimension ref="A1:AO46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD50"/>
+      <selection activeCell="A35" sqref="A34:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -978,40 +966,40 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="AF1" s="15"/>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="9"/>
@@ -1020,16 +1008,16 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="9"/>
@@ -1038,16 +1026,16 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="9"/>
@@ -1056,16 +1044,16 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="9"/>
@@ -1074,16 +1062,16 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="9"/>
@@ -1092,16 +1080,16 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="9"/>
@@ -1110,16 +1098,16 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="9"/>
@@ -1128,16 +1116,16 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="9"/>
@@ -1146,16 +1134,16 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="14"/>
@@ -1164,36 +1152,36 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G11" s="8"/>
       <c r="AF11" s="15"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="8"/>
@@ -1202,36 +1190,36 @@
     </row>
     <row r="13" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF13" s="15"/>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="8"/>
@@ -1240,167 +1228,167 @@
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G15" s="8"/>
       <c r="AF15" s="15"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF16" s="15"/>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G17" s="8"/>
       <c r="AF17" s="15"/>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF18" s="15"/>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF19" s="15"/>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF20" s="15"/>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G21" s="8"/>
       <c r="AF21" s="15"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF22" s="15"/>
     </row>
@@ -1409,19 +1397,19 @@
         <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G23" s="7"/>
       <c r="AF23" s="15"/>
@@ -1431,16 +1419,16 @@
         <v>7</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -1451,16 +1439,16 @@
         <v>8</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -1468,25 +1456,25 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF26" s="15"/>
     </row>
@@ -1495,22 +1483,22 @@
         <v>9</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF27" s="15"/>
     </row>
@@ -1519,17 +1507,17 @@
         <v>10</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G28" s="7"/>
       <c r="AF28" s="15"/>
@@ -1539,18 +1527,18 @@
         <v>11</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF29" s="15"/>
     </row>
@@ -1559,70 +1547,70 @@
         <v>12</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF30" s="15"/>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF31" s="15"/>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF32" s="15"/>
     </row>
@@ -1631,22 +1619,22 @@
         <v>13</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF33" s="15"/>
     </row>
@@ -1655,17 +1643,17 @@
         <v>14</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G34" s="7"/>
       <c r="AF34" s="15"/>
@@ -1675,83 +1663,79 @@
         <v>15</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AF35" s="15"/>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="B36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="F36" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G36" s="7"/>
+        <v>63</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="AF36" s="15"/>
     </row>
     <row r="37" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="A37" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
       <c r="AF37" s="15"/>
     </row>
     <row r="38" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="A38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
       <c r="AF38" s="15"/>
     </row>
     <row r="39" spans="1:41" x14ac:dyDescent="0.2">
@@ -1759,13 +1743,13 @@
         <v>29</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="10"/>
@@ -1777,13 +1761,13 @@
         <v>30</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="10"/>
@@ -1791,53 +1775,53 @@
       <c r="AF40" s="15"/>
     </row>
     <row r="41" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="10"/>
-      <c r="G41" s="10"/>
+      <c r="A41" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
       <c r="AF41" s="15"/>
     </row>
     <row r="42" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
+      <c r="A42" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
       <c r="AF42" s="15"/>
     </row>
     <row r="43" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E43" s="11"/>
       <c r="F43" s="12"/>
@@ -1846,16 +1830,16 @@
     </row>
     <row r="44" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="12"/>
@@ -1864,7 +1848,7 @@
     </row>
     <row r="45" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>35</v>
@@ -1873,7 +1857,7 @@
         <v>35</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="12"/>
@@ -1882,7 +1866,7 @@
     </row>
     <row r="46" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>35</v>
@@ -1891,57 +1875,21 @@
         <v>35</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="AF46" s="15"/>
-    </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="AF47" s="15"/>
-    </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="AF48" s="15"/>
-      <c r="AG48" s="4"/>
-      <c r="AH48" s="4"/>
-      <c r="AI48" s="4"/>
-      <c r="AJ48" s="4"/>
-      <c r="AK48" s="4"/>
-      <c r="AL48" s="4"/>
-      <c r="AM48" s="4"/>
-      <c r="AN48" s="4"/>
-      <c r="AO48" s="4"/>
+      <c r="AG46" s="4"/>
+      <c r="AH46" s="4"/>
+      <c r="AI46" s="4"/>
+      <c r="AJ46" s="4"/>
+      <c r="AK46" s="4"/>
+      <c r="AL46" s="4"/>
+      <c r="AM46" s="4"/>
+      <c r="AN46" s="4"/>
+      <c r="AO46" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1965,16 +1913,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>